<commit_message>
estatistica total de alocacoes
</commit_message>
<xml_diff>
--- a/SWAP2.xlsx
+++ b/SWAP2.xlsx
@@ -169,11 +169,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1536826866"/>
-        <c:axId val="1505613730"/>
+        <c:axId val="1946522055"/>
+        <c:axId val="1405036636"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1536826866"/>
+        <c:axId val="1946522055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -205,10 +205,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505613730"/>
+        <c:crossAx val="1405036636"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1505613730"/>
+        <c:axId val="1405036636"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -256,7 +256,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1536826866"/>
+        <c:crossAx val="1946522055"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -321,11 +321,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1575896342"/>
-        <c:axId val="454934717"/>
+        <c:axId val="934502762"/>
+        <c:axId val="26462670"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1575896342"/>
+        <c:axId val="934502762"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -357,10 +357,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="454934717"/>
+        <c:crossAx val="26462670"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="454934717"/>
+        <c:axId val="26462670"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +408,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1575896342"/>
+        <c:crossAx val="934502762"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>